<commit_message>
cleanup and added README for future work
</commit_message>
<xml_diff>
--- a/evaluation_files/evaluation_charts.xlsx
+++ b/evaluation_files/evaluation_charts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasceccarelli/Library/Mobile Documents/com~apple~CloudDocs/Research/respiratory_sound/evaluation_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasceccarelli/Documents/Archive/Research/CyberMed/cybermed_research/evaluation_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E93A86-0C7E-9249-B49B-37D60CC58694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E254191E-36C7-8840-930A-437972EBDEEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="19520" activeTab="3" xr2:uid="{D2F8ABD8-EFEF-3247-A4F2-5C54BC21D097}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19420" activeTab="1" xr2:uid="{D2F8ABD8-EFEF-3247-A4F2-5C54BC21D097}"/>
   </bookViews>
   <sheets>
     <sheet name="preprocess crackling" sheetId="1" r:id="rId1"/>
@@ -8820,18 +8820,18 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37407680320719794"/>
-          <c:y val="0.89798157023850267"/>
-          <c:w val="0.36028425584997165"/>
-          <c:h val="6.9409734109323287E-2"/>
+          <c:x val="0.59724585884460024"/>
+          <c:y val="3.2608695652173912E-2"/>
+          <c:w val="0.370712378740227"/>
+          <c:h val="7.3032922515120391E-2"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
+      <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -12838,7 +12838,8 @@
         <c:axId val="755641279"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
+          <c:max val="1.05"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -12950,18 +12951,18 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17372152445033529"/>
-          <c:y val="0.90885113545589413"/>
-          <c:w val="0.62752945616271683"/>
-          <c:h val="6.9409734109323287E-2"/>
+          <c:x val="0.23121270288975071"/>
+          <c:y val="0"/>
+          <c:w val="0.53757459422049858"/>
+          <c:h val="7.3480193256682813E-2"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
+      <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -15406,7 +15407,8 @@
         <c:axId val="755641279"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
+          <c:max val="1.05"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -15525,18 +15527,18 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17372152445033529"/>
-          <c:y val="0.90885113545589413"/>
-          <c:w val="0.62752945616271683"/>
-          <c:h val="6.9409734109323287E-2"/>
+          <c:x val="0.22957159464720348"/>
+          <c:y val="3.6880930351960235E-3"/>
+          <c:w val="0.54085664648318532"/>
+          <c:h val="6.6965024681183219E-2"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
+      <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -29812,8 +29814,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>310803</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>172358</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -30953,8 +30955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC093EE-463F-8947-8E4F-74FD48F41C9A}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="132" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A13" zoomScale="132" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31184,8 +31186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E56220F7-CAB5-5743-B338-A7468D00B041}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D47" sqref="D46:D47"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="140" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31686,7 +31688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B19E455-80F9-1849-A8BA-E9CE6954671F}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="A16:E16"/>
     </sheetView>
   </sheetViews>
@@ -31964,7 +31966,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+      <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>